<commit_message>
Fix CSV Example File
</commit_message>
<xml_diff>
--- a/data/Relatório.xlsx
+++ b/data/Relatório.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Gráficos" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Relatório Geral" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Relatório" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Planilha4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Validação" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Relatório!$A$1:$P$11</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Relatório Geral'!$G$2:$K$1048576</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Relatório!$A:$P</definedName>
   </definedNames>
@@ -1240,11 +1240,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="3062515"/>
-        <c:axId val="6998898"/>
+        <c:axId val="21265503"/>
+        <c:axId val="70285004"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="3062515"/>
+        <c:axId val="21265503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6998898"/>
+        <c:crossAx val="70285004"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1308,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6998898"/>
+        <c:axId val="70285004"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1373,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3062515"/>
+        <c:crossAx val="21265503"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1815,11 +1815,11 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="-80"/>
-        <c:axId val="86881000"/>
-        <c:axId val="52502631"/>
+        <c:axId val="4842608"/>
+        <c:axId val="38511998"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86881000"/>
+        <c:axId val="4842608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52502631"/>
+        <c:crossAx val="38511998"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52502631"/>
+        <c:axId val="38511998"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1948,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86881000"/>
+        <c:crossAx val="4842608"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3205,11 +3205,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="83205046"/>
-        <c:axId val="93888733"/>
+        <c:axId val="97035152"/>
+        <c:axId val="2611696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83205046"/>
+        <c:axId val="97035152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3265,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93888733"/>
+        <c:crossAx val="2611696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3273,7 +3273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93888733"/>
+        <c:axId val="2611696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3338,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83205046"/>
+        <c:crossAx val="97035152"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3400,9 +3400,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795960</xdr:colOff>
+      <xdr:colOff>795600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3411,7 +3411,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="1905480"/>
-        <a:ext cx="6550200" cy="3555000"/>
+        <a:ext cx="6549840" cy="3554640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3430,9 +3430,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795960</xdr:colOff>
+      <xdr:colOff>795600</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3441,7 +3441,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="9728640"/>
-        <a:ext cx="6550200" cy="4455000"/>
+        <a:ext cx="6549840" cy="4454640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3460,9 +3460,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795960</xdr:colOff>
+      <xdr:colOff>795600</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3471,7 +3471,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="5714280"/>
-        <a:ext cx="6550200" cy="3551400"/>
+        <a:ext cx="6549840" cy="3551040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4368,7 +4368,7 @@
       <c r="E22" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E22"/>
+  <autoFilter ref="A2:E21"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.252083333333333" right="0.252083333333333" top="0.489583333333333" bottom="0.489583333333333" header="0.252083333333333" footer="0.252083333333333"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4388,7 +4388,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4994,23 +4994,23 @@
   <autoFilter ref="A1:P11"/>
   <dataValidations count="5">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H500" type="list">
-      <formula1>Planilha4!$A$2:$A$3</formula1>
+      <formula1>Validação!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L500" type="list">
-      <formula1>Planilha4!$B$2:$B$3</formula1>
+      <formula1>Validação!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2:M500" type="list">
-      <formula1>Planilha4!$C$2:$C$3</formula1>
+      <formula1>Validação!$C$2:$C$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O2:O500" type="list">
-      <formula1>Planilha4!$D$2:$D$6</formula1>
+      <formula1>Validação!$D$2:$D$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:P500" type="list">
-      <formula1>Planilha4!$E$2:$E$4</formula1>
+      <formula1>Validação!$E$2:$E$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix Marker Bug and Data Parser
</commit_message>
<xml_diff>
--- a/data/Relatório.xlsx
+++ b/data/Relatório.xlsx
@@ -5,18 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Gráficos" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Relatório Geral" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Relatório" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Validação" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Validação" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Relatório!$A$1:$P$11</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Relatório Geral'!$G$2:$K$1048576</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Relatório!$A:$P</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="82">
   <si>
     <t xml:space="preserve">TOTAL DE CASOS</t>
   </si>
@@ -44,13 +44,13 @@
     <t xml:space="preserve">STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">Domicílio</t>
+    <t xml:space="preserve">Residência</t>
   </si>
   <si>
     <t xml:space="preserve">Descartado</t>
   </si>
   <si>
-    <t xml:space="preserve">Curado</t>
+    <t xml:space="preserve">Alta</t>
   </si>
   <si>
     <t xml:space="preserve">Suspeito</t>
@@ -62,13 +62,10 @@
     <t xml:space="preserve">Confirmado</t>
   </si>
   <si>
-    <t xml:space="preserve">UTI</t>
+    <t xml:space="preserve">Óbito</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Óbito</t>
   </si>
   <si>
     <t xml:space="preserve">Letalidade</t>
@@ -619,7 +616,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1240,11 +1237,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="21265503"/>
-        <c:axId val="70285004"/>
+        <c:axId val="23102671"/>
+        <c:axId val="53851676"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="21265503"/>
+        <c:axId val="23102671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1297,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70285004"/>
+        <c:crossAx val="53851676"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1308,7 +1305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70285004"/>
+        <c:axId val="53851676"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1370,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21265503"/>
+        <c:crossAx val="23102671"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1424,7 +1421,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1815,11 +1812,11 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="-80"/>
-        <c:axId val="4842608"/>
-        <c:axId val="38511998"/>
+        <c:axId val="81442283"/>
+        <c:axId val="75165992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4842608"/>
+        <c:axId val="81442283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1872,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38511998"/>
+        <c:crossAx val="75165992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38511998"/>
+        <c:axId val="75165992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1945,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4842608"/>
+        <c:crossAx val="81442283"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2009,7 +2006,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3205,11 +3202,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="97035152"/>
-        <c:axId val="2611696"/>
+        <c:axId val="84178276"/>
+        <c:axId val="45721178"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97035152"/>
+        <c:axId val="84178276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3262,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2611696"/>
+        <c:crossAx val="45721178"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3273,7 +3270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2611696"/>
+        <c:axId val="45721178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97035152"/>
+        <c:crossAx val="84178276"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3396,11 +3393,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795600</xdr:colOff>
+      <xdr:colOff>795240</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
@@ -3410,8 +3407,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="1905480"/>
-        <a:ext cx="6549840" cy="3554640"/>
+        <a:off x="0" y="1905840"/>
+        <a:ext cx="6549480" cy="3554280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3426,11 +3423,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795600</xdr:colOff>
+      <xdr:colOff>795240</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
@@ -3440,8 +3437,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="9728640"/>
-        <a:ext cx="6549840" cy="4454640"/>
+        <a:off x="0" y="9729000"/>
+        <a:ext cx="6549480" cy="4454280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3455,12 +3452,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>795600</xdr:colOff>
+      <xdr:colOff>795240</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
@@ -3470,8 +3467,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="5714280"/>
-        <a:ext cx="6549840" cy="3551040"/>
+        <a:off x="0" y="5714640"/>
+        <a:ext cx="6549480" cy="3550680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3497,10 +3494,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I49" activeCellId="0" sqref="I49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3570,7 +3567,7 @@
       </c>
       <c r="B6" s="5" t="n">
         <f aca="false">COUNTIF(Relatório!$O$2:$O$500,A6)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
@@ -3597,32 +3594,29 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <f aca="false">COUNTIF(Relatório!$O$2:$O$500,A8)</f>
-        <v>2</v>
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <f aca="false">SUM(B4:B7)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <f aca="false">SUM(B4:B8)</f>
-        <v>10</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="10" t="n">
-        <f aca="false">B8/E6</f>
+        <f aca="false">B7/E6</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="11"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
@@ -3665,42 +3659,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4368,7 +4362,7 @@
       <c r="E22" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E21"/>
+  <autoFilter ref="A2:E22"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.252083333333333" right="0.252083333333333" top="0.489583333333333" bottom="0.489583333333333" header="0.252083333333333" footer="0.252083333333333"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4387,8 +4381,8 @@
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4414,46 +4408,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>1</v>
@@ -4470,13 +4464,13 @@
         <v>43901</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="14" t="n">
         <v>43899</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="14" t="n">
         <v>18744</v>
@@ -4486,22 +4480,22 @@
         <v>68</v>
       </c>
       <c r="H2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>44</v>
-      </c>
       <c r="M2" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" s="16" t="n">
         <v>5</v>
@@ -4521,13 +4515,13 @@
         <v>43901</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="14" t="n">
         <v>43899</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="14" t="n">
         <v>17145</v>
@@ -4537,28 +4531,28 @@
         <v>73</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>49</v>
-      </c>
       <c r="M3" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="16" t="n">
         <v>5</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>9</v>
@@ -4572,13 +4566,13 @@
         <v>43905</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>43901</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="14" t="n">
         <v>20172</v>
@@ -4588,22 +4582,22 @@
         <v>65</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="L4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N4" s="16" t="n">
         <v>30</v>
@@ -4623,13 +4617,13 @@
         <v>43906</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="14" t="n">
         <v>43901</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="14" t="n">
         <v>28568</v>
@@ -4639,28 +4633,28 @@
         <v>42</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="L5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N5" s="16" t="n">
         <v>17</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P5" s="16" t="s">
         <v>9</v>
@@ -4674,13 +4668,13 @@
         <v>43907</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="14" t="n">
         <v>43903</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="14" t="n">
         <v>18777</v>
@@ -4690,22 +4684,22 @@
         <v>68</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="L6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="16" t="n">
         <v>19</v>
@@ -4725,13 +4719,13 @@
         <v>43906</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="14" t="n">
         <v>43905</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="14" t="n">
         <v>19299</v>
@@ -4741,22 +4735,22 @@
         <v>67</v>
       </c>
       <c r="H7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>66</v>
-      </c>
       <c r="L7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N7" s="16" t="n">
         <v>12</v>
@@ -4776,13 +4770,13 @@
         <v>43907</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="14" t="n">
         <v>43905</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="14" t="n">
         <v>21353</v>
@@ -4792,28 +4786,28 @@
         <v>61</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>70</v>
-      </c>
       <c r="L8" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" s="16" t="n">
         <v>10</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>9</v>
@@ -4827,13 +4821,13 @@
         <v>43908</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="14" t="n">
         <v>43904</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="14" t="n">
         <v>30633</v>
@@ -4843,28 +4837,28 @@
         <v>36</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I9" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="L9" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" s="16" t="n">
         <v>8</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>9</v>
@@ -4878,13 +4872,13 @@
         <v>43909</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="14" t="n">
         <v>43907</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="14" t="n">
         <v>31295</v>
@@ -4894,22 +4888,22 @@
         <v>34</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="L10" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N10" s="16" t="n">
         <v>6</v>
@@ -4929,13 +4923,13 @@
         <v>43911</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="14" t="n">
         <v>43906</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="14" t="n">
         <v>20445</v>
@@ -4945,22 +4939,22 @@
         <v>64</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="L11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N11" s="16" t="n">
         <v>18</v>
@@ -5033,7 +5027,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5047,13 +5041,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -5064,13 +5058,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -5081,13 +5075,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -5098,7 +5092,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -5106,13 +5100,11 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D6" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix: Method calls and sample files
- Simplification of method calls
- Correction of sample files
</commit_message>
<xml_diff>
--- a/data/Relatório.xlsx
+++ b/data/Relatório.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gráficos" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,8 +15,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Relatório!$A$1:$P$11</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Relatório Geral'!$A$2:$E$22</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Relatório Geral'!$G$2:$K$1048576</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Relatório!$A:$P</definedName>
   </definedNames>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">Feminino</t>
   </si>
   <si>
-    <t xml:space="preserve">Silva Jardim, 92, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Silva Jardim, 92, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">Itapetininga</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">Maitê Beatriz Lúcia Gomes</t>
   </si>
   <si>
-    <t xml:space="preserve">General Carneiro, 476, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Gal. Carneiro, 476, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 2698-8159</t>
@@ -197,7 +197,7 @@
     <t xml:space="preserve">Lúcia Benedita Baptista</t>
   </si>
   <si>
-    <t xml:space="preserve">Professor Francisco Valio, 378, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Professor Francisco Valio, 378, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 3954-2818</t>
@@ -209,7 +209,7 @@
     <t xml:space="preserve">Eliane Silvana Malu Almeida</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Doutor Virgílio de Rezende, 29, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Rua Doutor Virgílio de Rezende, 29, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 3852-3052</t>
@@ -224,7 +224,7 @@
     <t xml:space="preserve">Masculino</t>
   </si>
   <si>
-    <t xml:space="preserve">Benjamin Constant, 188, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Benjamin Constant, 188, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 2814-4252</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">Cláudia Mariah Lopes</t>
   </si>
   <si>
-    <t xml:space="preserve">Coronel Clementino Matias de Oliveira, 30, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Coronel Clementino Matias de Oliveira, 30, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 2995-9114</t>
@@ -248,7 +248,7 @@
     <t xml:space="preserve">Pedro Henrique Bryan Araújo</t>
   </si>
   <si>
-    <t xml:space="preserve">Monsenhor Soares, 39, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Monsenhor Soares, 39, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 3628-0319</t>
@@ -260,7 +260,7 @@
     <t xml:space="preserve">Igor Tiago Brito</t>
   </si>
   <si>
-    <t xml:space="preserve">Campos Salles, 217, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Campos Salles, 217, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 3794-7422</t>
@@ -272,7 +272,7 @@
     <t xml:space="preserve">Erick Cauã Pietro Costa</t>
   </si>
   <si>
-    <t xml:space="preserve">Saldanha Marinho, 241, Centro, Itapetininga, São Paulo</t>
+    <t xml:space="preserve">Rua Saldanha Marinho, 241, Centro, Itapetininga, São Paulo</t>
   </si>
   <si>
     <t xml:space="preserve">(15) 2525-0325</t>
@@ -616,7 +616,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -636,7 +636,7 @@
               <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Casos Acumulados por Faixa Etária</a:t>
+              <a:t>Casos Diários</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -644,164 +644,22 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Relatório Geral'!$K$2:$K$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ÓBITOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Relatório Geral'!$I$3:$I$15</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0-9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10-19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30-39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40-49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50-59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>60-69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>70-79</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>80-89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90-99</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100-109</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>110-119</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>120-129</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Relatório Geral'!$K$3:$K$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Relatório Geral'!$J$2:$J$2</c:f>
+              <c:f>'Relatório Geral'!$B$2:$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -814,154 +672,506 @@
             <a:solidFill>
               <a:srgbClr val="729fcf"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="729fcf"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="729fcf"/>
               </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
             </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="729fcf"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
+          </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:numFmt formatCode="General" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:numFmt formatCode="General" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Relatório Geral'!$I$3:$I$15</c:f>
+              <c:f>'Relatório Geral'!$A$3:$A$150</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
-                  <c:v>0-9</c:v>
+                  <c:v>01/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10-19</c:v>
+                  <c:v>02/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20-29</c:v>
+                  <c:v>03/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30-39</c:v>
+                  <c:v>04/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40-49</c:v>
+                  <c:v>05/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50-59</c:v>
+                  <c:v>06/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60-69</c:v>
+                  <c:v>07/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70-79</c:v>
+                  <c:v>08/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80-89</c:v>
+                  <c:v>09/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90-99</c:v>
+                  <c:v>10/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100-109</c:v>
+                  <c:v>11/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110-119</c:v>
+                  <c:v>12/03/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120-129</c:v>
+                  <c:v>13/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Relatório Geral'!$J$3:$J$15</c:f>
+              <c:f>'Relatório Geral'!$B$3:$B$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -975,43 +1185,68 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:gapWidth val="0"/>
-        <c:overlap val="-80"/>
-        <c:axId val="4243728"/>
-        <c:axId val="54231563"/>
-      </c:barChart>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="96953633"/>
+        <c:axId val="84925334"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="4243728"/>
+        <c:axId val="96953633"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1255,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1032,7 +1267,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Idades</a:t>
+                  <a:t>Dias</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1040,17 +1275,17 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -1067,7 +1302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54231563"/>
+        <c:crossAx val="84925334"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1075,7 +1310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54231563"/>
+        <c:axId val="84925334"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,7 +1318,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -1093,7 +1328,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1113,17 +1348,17 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -1140,13 +1375,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4243728"/>
+        <c:crossAx val="96953633"/>
         <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -1155,20 +1390,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.809182052265381"/>
-          <c:y val="0.442000966650556"/>
-          <c:w val="0.171433267587114"/>
-          <c:h val="0.087569483605897"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -1201,7 +1426,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1221,7 +1446,7 @@
               <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Casos Diários Acumulados</a:t>
+              <a:t>Casos Acumulados por Faixa Etária</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1229,22 +1454,169 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Relatório Geral'!$B$2:$B$2</c:f>
+              <c:f>'Relatório Geral'!$K$2:$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ÓBITOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Relatório Geral'!$I$3:$I$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40-49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50-59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60-69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70-79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80-89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90-99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100-109</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110-119</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120-129</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Relatório Geral'!$K$3:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Relatório Geral'!$J$2:$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1257,501 +1629,159 @@
             <a:solidFill>
               <a:srgbClr val="729fcf"/>
             </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="729fcf"/>
-              </a:solidFill>
-              <a:round/>
+            <a:ln w="0">
+              <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="729fcf"/>
               </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
             </c:spPr>
-          </c:marker>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="729fcf"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
+                    <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Relatório Geral'!$A$3:$A$150</c:f>
+              <c:f>'Relatório Geral'!$I$3:$I$15</c:f>
               <c:strCache>
-                <c:ptCount val="148"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>01/03/2020</c:v>
+                  <c:v>0-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>02/03/2020</c:v>
+                  <c:v>10-19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>03/03/2020</c:v>
+                  <c:v>20-29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>04/03/2020</c:v>
+                  <c:v>30-39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>05/03/2020</c:v>
+                  <c:v>40-49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>06/03/2020</c:v>
+                  <c:v>50-59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>07/03/2020</c:v>
+                  <c:v>60-69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>08/03/2020</c:v>
+                  <c:v>70-79</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>09/03/2020</c:v>
+                  <c:v>80-89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10/03/2020</c:v>
+                  <c:v>90-99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11/03/2020</c:v>
+                  <c:v>100-109</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12/03/2020</c:v>
+                  <c:v>110-119</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v/>
+                  <c:v>120-129</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Relatório Geral'!$D$3:$D$150</c:f>
+              <c:f>'Relatório Geral'!$J$3:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1765,13 +1795,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1789,619 +1819,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Relatório Geral'!$C$2:$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ÓBITOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Relatório Geral'!$A$3:$A$150</c:f>
-              <c:strCache>
-                <c:ptCount val="148"/>
-                <c:pt idx="0">
-                  <c:v>01/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>02/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>03/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>04/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>05/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>06/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>07/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>08/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>09/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19/03/2020</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Relatório Geral'!$E$3:$E$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:axId val="19638367"/>
-        <c:axId val="70002578"/>
-      </c:lineChart>
+        <c:gapWidth val="0"/>
+        <c:overlap val="-80"/>
+        <c:axId val="27850882"/>
+        <c:axId val="36605309"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="19638367"/>
+        <c:axId val="27850882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,7 +1840,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0"/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2422,7 +1852,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Dias</a:t>
+                  <a:t>Idades</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2430,17 +1860,17 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -2457,7 +1887,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70002578"/>
+        <c:crossAx val="36605309"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2465,7 +1895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70002578"/>
+        <c:axId val="36605309"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2473,7 +1903,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -2483,7 +1913,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr rot="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2503,7 +1933,7 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
@@ -2513,7 +1943,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -2530,13 +1960,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19638367"/>
+        <c:crossAx val="27850882"/>
         <c:crossesAt val="1"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -2545,10 +1975,20 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.809182052265381"/>
+          <c:y val="0.442000966650556"/>
+          <c:w val="0.171433267587114"/>
+          <c:h val="0.087569483605897"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -2581,7 +2021,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2601,7 +2041,7 @@
               <a:rPr b="1" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Casos Diários</a:t>
+              <a:t>Casos Diários Acumulados</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2609,7 +2049,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -2655,7 +2095,7 @@
           </c:marker>
           <c:dLbls>
             <c:txPr>
-              <a:bodyPr/>
+              <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2673,6 +2113,11 @@
             <c:showPercent val="0"/>
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3128,7 +2573,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Relatório Geral'!$B$3:$B$150</c:f>
+              <c:f>'Relatório Geral'!$D$3:$D$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="148"/>
@@ -3172,22 +2617,602 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Relatório Geral'!$C$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ÓBITOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Relatório Geral'!$A$3:$A$150</c:f>
+              <c:strCache>
+                <c:ptCount val="148"/>
+                <c:pt idx="0">
+                  <c:v>01/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>03/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>04/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>05/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>06/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>07/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>08/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>09/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19/03/2020</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Relatório Geral'!$E$3:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3196,17 +3221,17 @@
         </c:ser>
         <c:hiLowLines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="29707516"/>
-        <c:axId val="36998496"/>
+        <c:axId val="7400457"/>
+        <c:axId val="73064832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29707516"/>
+        <c:axId val="7400457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3235,17 +3260,17 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -3262,7 +3287,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36998496"/>
+        <c:crossAx val="73064832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3270,7 +3295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36998496"/>
+        <c:axId val="73064832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3278,7 +3303,7 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
@@ -3308,17 +3333,17 @@
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
-            <a:ln>
+            <a:ln w="0">
               <a:noFill/>
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
@@ -3335,13 +3360,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29707516"/>
+        <c:crossAx val="7400457"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="b3b3b3"/>
           </a:solidFill>
@@ -3353,7 +3378,7 @@
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -3397,9 +3422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>794520</xdr:colOff>
+      <xdr:colOff>794160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3408,7 +3433,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="1905840"/>
-        <a:ext cx="6548760" cy="3553560"/>
+        <a:ext cx="6548400" cy="3553200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3427,9 +3452,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>794520</xdr:colOff>
+      <xdr:colOff>794160</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3438,7 +3463,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="9729000"/>
-        <a:ext cx="6548760" cy="4453560"/>
+        <a:ext cx="6548400" cy="4453200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3457,9 +3482,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>794520</xdr:colOff>
+      <xdr:colOff>794160</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3468,7 +3493,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="5714640"/>
-        <a:ext cx="6548760" cy="3549960"/>
+        <a:ext cx="6548400" cy="3549600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3490,13 +3515,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -3631,7 +3656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -4362,7 +4387,7 @@
       <c r="E22" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E22"/>
+  <autoFilter ref="A2:E21"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.252083333333333" right="0.252083333333333" top="0.489583333333333" bottom="0.489583333333333" header="0.252083333333333" footer="0.252083333333333"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4375,14 +4400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4403,7 +4428,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4477,12 +4502,12 @@
       </c>
       <c r="G2" s="15" t="n">
         <f aca="true">IF(F2,INT((TODAY()-F2)/365.25),"")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J2" s="16" t="s">
@@ -4584,7 +4609,7 @@
       <c r="H4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J4" s="16" t="s">
@@ -4635,7 +4660,7 @@
       <c r="H5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J5" s="16" t="s">
@@ -4681,12 +4706,12 @@
       </c>
       <c r="G6" s="15" t="n">
         <f aca="true">IF(F6,INT((TODAY()-F6)/365.25),"")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J6" s="16" t="s">
@@ -4732,12 +4757,12 @@
       </c>
       <c r="G7" s="15" t="n">
         <f aca="true">IF(F7,INT((TODAY()-F7)/365.25),"")</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="J7" s="16" t="s">
@@ -4783,12 +4808,12 @@
       </c>
       <c r="G8" s="15" t="n">
         <f aca="true">IF(F8,INT((TODAY()-F8)/365.25),"")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="J8" s="16" t="s">
@@ -4834,12 +4859,12 @@
       </c>
       <c r="G9" s="15" t="n">
         <f aca="true">IF(F9,INT((TODAY()-F9)/365.25),"")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J9" s="16" t="s">
@@ -4885,12 +4910,12 @@
       </c>
       <c r="G10" s="15" t="n">
         <f aca="true">IF(F10,INT((TODAY()-F10)/365.25),"")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J10" s="16" t="s">
@@ -4941,7 +4966,7 @@
       <c r="H11" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J11" s="16" t="s">
@@ -5020,7 +5045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>

</xml_diff>